<commit_message>
Added all direction animations, colors, removed buttons and enabled swipe actions again
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Android\Projects\2.2048\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF6EB71-B7B8-48DF-992A-C9EA4980A670}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3335510-20D3-4EA2-8E73-0EF573057223}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{44A1CE25-EE5E-4491-9340-CFF7A6FF5C1B}"/>
   </bookViews>
@@ -30,57 +30,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Blank</t>
-  </si>
-  <si>
-    <t>#008000</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Green</t>
   </si>
   <si>
-    <t>Cyan</t>
-  </si>
-  <si>
-    <t>#40E0D0</t>
-  </si>
-  <si>
-    <t>Turquoise</t>
-  </si>
-  <si>
-    <t>#800000</t>
-  </si>
-  <si>
     <t>Maroon</t>
   </si>
   <si>
-    <t>#e22a64</t>
-  </si>
-  <si>
-    <t>#672ae2</t>
-  </si>
-  <si>
-    <t>#2abde2</t>
-  </si>
-  <si>
-    <t>#cfe22a</t>
-  </si>
-  <si>
-    <t>#e29e2a</t>
-  </si>
-  <si>
-    <t>#e2582a</t>
-  </si>
-  <si>
-    <t>#2ae2d5</t>
-  </si>
-  <si>
-    <t>Added</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>val</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>arr</t>
+  </si>
+  <si>
+    <t>mov</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#8504ef</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>#ef0462</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>#1b9633</t>
+  </si>
+  <si>
+    <t>#1c7db5</t>
+  </si>
+  <si>
+    <t>Sky Blue Dark</t>
+  </si>
+  <si>
+    <t>#99471e</t>
+  </si>
+  <si>
+    <t>#991e1e</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>#4f0541</t>
+  </si>
+  <si>
+    <t>Dark Purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dark Brown</t>
+  </si>
+  <si>
+    <t>#686222</t>
+  </si>
+  <si>
+    <t>Dark Yellow</t>
+  </si>
+  <si>
+    <t>#635f5f</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>#005600</t>
+  </si>
+  <si>
+    <t>Dark Green</t>
+  </si>
+  <si>
+    <t>#0021f9</t>
   </si>
 </sst>
 </file>
@@ -124,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,6 +202,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,477 +521,649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2288CD-F746-4F6C-808B-CA6747BD3287}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" style="1"/>
     <col min="3" max="4" width="15.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="15.7109375" style="1"/>
+    <col min="7" max="7" width="15.7109375" style="4" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="15.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+    <row r="1" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4">
+        <f>LOG(B3, 2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <f>B3*2</f>
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" ref="G4:G13" si="0">LOG(B4, 2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:B13" si="1">B4*2</f>
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4">
-        <f>LOG(B2, 2)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <f>B2*2</f>
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4">
-        <f t="shared" ref="E3:E12" si="0">LOG(B3, 2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" ref="B4:B12" si="1">B3*2</f>
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
+        <v>2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>3</v>
+      </c>
+      <c r="O6" s="1">
         <v>4</v>
       </c>
-      <c r="L5" s="1">
-        <f>MOD(G5-1,4)</f>
+      <c r="Q6" s="1">
+        <f>MOD(L6-1,4)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="1">
-        <f t="shared" ref="M5:O5" si="2">MOD(H5-1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="R6" s="1">
+        <f t="shared" ref="R6:T6" si="2">MOD(M6-1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="T6" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="1">
+      <c r="L7" s="1">
         <v>5</v>
       </c>
-      <c r="H6" s="1">
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="I6" s="1">
+      <c r="N7" s="1">
         <v>7</v>
       </c>
-      <c r="J6" s="1">
+      <c r="O7" s="1">
         <v>8</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" ref="L6:L8" si="3">MOD(G6-1,4)</f>
+      <c r="Q7" s="1">
+        <f t="shared" ref="Q7:Q9" si="3">MOD(L7-1,4)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="1">
-        <f t="shared" ref="M6:M8" si="4">MOD(H6-1,4)</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <f t="shared" ref="N6:N8" si="5">MOD(I6-1,4)</f>
-        <v>2</v>
-      </c>
-      <c r="O6" s="1">
-        <f t="shared" ref="O6:O8" si="6">MOD(J6-1,4)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="R7" s="1">
+        <f t="shared" ref="R7:R9" si="4">MOD(M7-1,4)</f>
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" ref="S7:S9" si="5">MOD(N7-1,4)</f>
+        <v>2</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" ref="T7:T9" si="6">MOD(O7-1,4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G7" s="1">
+      <c r="L8" s="1">
         <v>9</v>
       </c>
-      <c r="H7" s="1">
+      <c r="M8" s="1">
         <v>10</v>
       </c>
-      <c r="I7" s="1">
+      <c r="N8" s="1">
         <v>11</v>
       </c>
-      <c r="J7" s="1">
+      <c r="O8" s="1">
         <v>12</v>
       </c>
-      <c r="L7" s="1">
+      <c r="Q8" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M7" s="1">
+      <c r="R8" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N7" s="1">
+      <c r="S8" s="1">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="O7" s="1">
+      <c r="T8" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="9" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G8" s="1">
+      <c r="L9" s="1">
         <v>13</v>
       </c>
-      <c r="H8" s="1">
+      <c r="M9" s="1">
         <v>14</v>
       </c>
-      <c r="I8" s="1">
+      <c r="N9" s="1">
         <v>15</v>
       </c>
-      <c r="J8" s="1">
-        <v>16</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="O9" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q9" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M8" s="1">
+      <c r="R9" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N8" s="1">
+      <c r="S9" s="1">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="O8" s="1">
+      <c r="T9" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
-        <f t="shared" si="1"/>
+      <c r="B11" s="1">
+        <f>B10*2</f>
         <v>512</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <f t="shared" si="1"/>
         <v>1024</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="1">
-        <v>3</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1">
+        <v>2</v>
+      </c>
+      <c r="N12" s="1">
+        <v>3</v>
+      </c>
+      <c r="O12" s="1">
         <v>4</v>
       </c>
-      <c r="L11" s="3">
-        <f>CEILING(G11/4, 1)-1</f>
+      <c r="Q12" s="3">
+        <f>CEILING(L12/4, 1)-1</f>
         <v>0</v>
       </c>
-      <c r="M11" s="3">
-        <f t="shared" ref="M11:O14" si="7">CEILING(H11/4, 1)-1</f>
+      <c r="R12" s="3">
+        <f t="shared" ref="R12:T15" si="7">CEILING(M12/4, 1)-1</f>
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="S12" s="3">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="O11" s="3">
+      <c r="T12" s="3">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="13" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G12" s="1">
+      <c r="L13" s="1">
         <v>5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="M13" s="1">
         <v>6</v>
       </c>
-      <c r="I12" s="1">
+      <c r="N13" s="1">
         <v>7</v>
       </c>
-      <c r="J12" s="1">
+      <c r="O13" s="1">
         <v>8</v>
       </c>
-      <c r="L12" s="3">
-        <f>CEILING(G12/4, 1)-1</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="3">
+      <c r="Q13" s="3">
+        <f>CEILING(L13/4, 1)-1</f>
+        <v>1</v>
+      </c>
+      <c r="R13" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="N12" s="3">
+      <c r="S13" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="O12" s="3">
+      <c r="T13" s="3">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G13" s="1">
+    <row r="14" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="1">
         <v>9</v>
       </c>
-      <c r="H13" s="1">
+      <c r="M14" s="1">
         <v>10</v>
       </c>
-      <c r="I13" s="1">
+      <c r="N14" s="1">
         <v>11</v>
       </c>
-      <c r="J13" s="1">
+      <c r="O14" s="1">
         <v>12</v>
       </c>
-      <c r="L13" s="3">
-        <f>CEILING(G13/4, 1)-1</f>
-        <v>2</v>
-      </c>
-      <c r="M13" s="3">
+      <c r="Q14" s="3">
+        <f>CEILING(L14/4, 1)-1</f>
+        <v>2</v>
+      </c>
+      <c r="R14" s="3">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="N13" s="3">
+      <c r="S14" s="3">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="O13" s="3">
+      <c r="T14" s="3">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="1">
+    <row r="15" spans="1:20" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="1">
         <v>13</v>
       </c>
-      <c r="H14" s="1">
+      <c r="M15" s="1">
         <v>14</v>
       </c>
-      <c r="I14" s="1">
+      <c r="N15" s="1">
         <v>15</v>
       </c>
-      <c r="J14" s="1">
-        <v>16</v>
-      </c>
-      <c r="L14" s="3">
-        <f>CEILING(G14/4, 1)-1</f>
-        <v>3</v>
-      </c>
-      <c r="M14" s="3">
+      <c r="O15" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="3">
+        <f>CEILING(L15/4, 1)-1</f>
+        <v>3</v>
+      </c>
+      <c r="R15" s="3">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="N14" s="3">
+      <c r="S15" s="3">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="O14" s="3">
+      <c r="T15" s="3">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="5:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G21" s="5">
+    <row r="21" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>3</v>
+      </c>
+      <c r="O21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="5">
+        <v>3</v>
+      </c>
+      <c r="M22" s="5">
+        <v>2</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="5">
         <v>0</v>
       </c>
-      <c r="H21" s="5">
-        <v>1</v>
-      </c>
-      <c r="I21" s="5">
-        <v>2</v>
-      </c>
-      <c r="J21" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="5:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="5:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="5:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="1">
-        <v>3</v>
+    </row>
+    <row r="23" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2</v>
+      </c>
+      <c r="O23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="4">
+        <v>3</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>4</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Swipes, added - Score, Undo etc.
</commit_message>
<xml_diff>
--- a/Colors.xlsx
+++ b/Colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Android\Projects\2.2048\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3335510-20D3-4EA2-8E73-0EF573057223}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84333AC6-3CEC-4613-A12A-58D0D5A29C2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{44A1CE25-EE5E-4491-9340-CFF7A6FF5C1B}"/>
   </bookViews>
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A2288CD-F746-4F6C-808B-CA6747BD3287}">
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1084,27 +1084,25 @@
     </row>
     <row r="22" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L22" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M22" s="5">
         <v>2</v>
       </c>
       <c r="N22" s="5">
-        <v>1</v>
-      </c>
-      <c r="O22" s="5">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="1">
-        <v>2</v>
+      <c r="N23" s="1">
+        <v>8</v>
       </c>
       <c r="O23" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,9 +1121,6 @@
       <c r="H24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O24" s="1">
-        <v>4</v>
-      </c>
     </row>
     <row r="25" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -1142,9 +1137,6 @@
       </c>
       <c r="H25" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="O25" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>